<commit_message>
Final Bucket Attachment Features + Update Tasks
</commit_message>
<xml_diff>
--- a/ZZ_Docs/Tasks.xlsx
+++ b/ZZ_Docs/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chalmers\2020\PPU080 Advanced computer aided design\06 - Project\PPU080_Excavator\ZZ_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBAE776-00B0-4F48-B377-929A080E0525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44865690-5489-459D-BE7B-D4C1972A82D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F51A760-8785-45A1-A29B-AFB17A55C109}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
   <si>
     <t xml:space="preserve">Group 18 </t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>Machining</t>
+  </si>
+  <si>
+    <t>Create 4 of them and assemble</t>
   </si>
 </sst>
 </file>
@@ -339,12 +342,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -357,6 +357,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -673,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780EFD92-2DE3-4928-85FB-6DCD7360F672}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -684,7 +699,7 @@
     <col min="1" max="1" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
@@ -704,42 +719,42 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="9">
         <f>SUM(D10)/1</f>
         <v>100</v>
       </c>
@@ -748,21 +763,21 @@
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="D10" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="9">
         <f>SUM(D12:D15)/4</f>
         <v>100</v>
       </c>
@@ -771,7 +786,7 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="7">
         <v>100</v>
       </c>
     </row>
@@ -779,7 +794,7 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="7">
         <v>100</v>
       </c>
     </row>
@@ -787,7 +802,7 @@
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="7">
         <v>100</v>
       </c>
     </row>
@@ -795,101 +810,101 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="D15" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="9">
         <f>SUM(D18:D24)/7</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="1">
-        <v>0</v>
+      <c r="D18" s="7">
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="1">
-        <v>0</v>
+      <c r="D19" s="7">
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="1">
-        <v>0</v>
+      <c r="D20" s="7">
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="1">
-        <v>0</v>
+      <c r="D21" s="7">
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="1">
-        <v>0</v>
+      <c r="D22" s="7">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="1">
-        <v>0</v>
+      <c r="D23" s="7">
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="D24" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="9">
         <f>SUM(D26:D29)/4</f>
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="7">
         <v>100</v>
       </c>
     </row>
@@ -897,7 +912,7 @@
       <c r="B27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="7">
         <v>100</v>
       </c>
     </row>
@@ -905,29 +920,29 @@
       <c r="B28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="1">
-        <v>0</v>
+      <c r="D28" s="7">
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="D29" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="9">
         <f>SUM(D31:D33)/3</f>
         <v>30</v>
       </c>
@@ -936,7 +951,7 @@
       <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="7">
         <v>0</v>
       </c>
     </row>
@@ -944,7 +959,7 @@
       <c r="B32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="7">
         <v>90</v>
       </c>
     </row>
@@ -952,21 +967,21 @@
       <c r="B33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="D33" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="9">
         <f>SUM(D35:D36)/2</f>
         <v>0</v>
       </c>
@@ -975,7 +990,7 @@
       <c r="B35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="7">
         <v>0</v>
       </c>
     </row>
@@ -983,30 +998,30 @@
       <c r="B36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="D36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="5">
-        <f>SUM(D38:D39)/2</f>
-        <v>100</v>
+      <c r="D37" s="9">
+        <f>SUM(D38:D40)/3</f>
+        <v>66.666666666666671</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="7">
         <v>100</v>
       </c>
     </row>
@@ -1014,242 +1029,250 @@
       <c r="B39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="D39" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="5">
-        <f>SUM(D41:D44)/4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41" s="1">
+      <c r="D41" s="9">
+        <f>SUM(D42:D45)/4</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="1">
+        <v>46</v>
+      </c>
+      <c r="D42" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" s="1">
+        <v>47</v>
+      </c>
+      <c r="D43" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="D45" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C46" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="5">
-        <f>SUM(D46:D48)/3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="1">
+      <c r="D46" s="9">
+        <f>SUM(D47:D49)/3</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D47" s="1">
+        <v>52</v>
+      </c>
+      <c r="D47" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+      <c r="D49" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C50" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D49" s="5">
-        <f>SUM(D50:D51)/2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4" t="s">
+      <c r="D50" s="9">
+        <f>SUM(D51:D52)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="3"/>
+      <c r="D51" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+      <c r="D52" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B53" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C53" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="5"/>
-    </row>
-    <row r="53" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
+      <c r="D53" s="9"/>
+    </row>
+    <row r="54" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C54" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D53" s="5"/>
-    </row>
-    <row r="54" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+      <c r="D54" s="9"/>
+    </row>
+    <row r="55" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B55" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C55" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D54" s="5"/>
-    </row>
-    <row r="55" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
+      <c r="D55" s="9"/>
+    </row>
+    <row r="56" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B56" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C56" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D55" s="5"/>
-    </row>
-    <row r="56" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
+      <c r="D56" s="9"/>
+    </row>
+    <row r="57" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B57" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C57" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D56" s="5"/>
-    </row>
-    <row r="57" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+      <c r="D57" s="9"/>
+    </row>
+    <row r="58" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B58" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C58" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D57" s="5"/>
-    </row>
-    <row r="58" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B59" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C59" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D58" s="5"/>
-    </row>
-    <row r="59" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
+      <c r="D59" s="9"/>
+    </row>
+    <row r="60" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B60" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C60" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D59" s="5"/>
-    </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
+      <c r="D60" s="9"/>
+    </row>
+    <row r="61" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B61" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C61" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D60" s="5"/>
+      <c r="D61" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D5:F6"/>
   </mergeCells>
-  <conditionalFormatting sqref="D12:D15 D10 D18:D24 D26:D29 D31:D33 D35:D36 D38:D39 D41:D44 D46:D48 D50:D51">
+  <conditionalFormatting sqref="D12:D15 D10 D18:D24 D26:D29 D31:D33 D35:D36 D38:D40 D42:D45 D47:D49 D51:D52">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Questions + Tasks Update + Bucket's Teeth
</commit_message>
<xml_diff>
--- a/ZZ_Docs/Tasks.xlsx
+++ b/ZZ_Docs/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chalmers\2020\PPU080 Advanced computer aided design\06 - Project\PPU080_Excavator\ZZ_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44865690-5489-459D-BE7B-D4C1972A82D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8F6F32-3C65-40C7-87CF-2ECECC76BBCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F51A760-8785-45A1-A29B-AFB17A55C109}"/>
   </bookViews>
@@ -182,9 +182,6 @@
     <t>Boom</t>
   </si>
   <si>
-    <t>Boom Attachment</t>
-  </si>
-  <si>
     <t>Task 8</t>
   </si>
   <si>
@@ -276,6 +273,9 @@
   </si>
   <si>
     <t>Create 4 of them and assemble</t>
+  </si>
+  <si>
+    <t>Boom's Attachment</t>
   </si>
 </sst>
 </file>
@@ -359,9 +359,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -372,6 +369,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -690,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780EFD92-2DE3-4928-85FB-6DCD7360F672}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -699,7 +699,7 @@
     <col min="1" max="1" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
@@ -719,16 +719,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -740,8 +740,8 @@
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>59</v>
+      <c r="D8" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -752,9 +752,9 @@
         <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="9">
+        <v>59</v>
+      </c>
+      <c r="D9" s="8">
         <f>SUM(D10)/1</f>
         <v>100</v>
       </c>
@@ -763,7 +763,7 @@
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>100</v>
       </c>
     </row>
@@ -775,9 +775,9 @@
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="9">
+        <v>59</v>
+      </c>
+      <c r="D11" s="8">
         <f>SUM(D12:D15)/4</f>
         <v>100</v>
       </c>
@@ -786,7 +786,7 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>100</v>
       </c>
     </row>
@@ -794,7 +794,7 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>100</v>
       </c>
     </row>
@@ -802,7 +802,7 @@
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>100</v>
       </c>
     </row>
@@ -810,7 +810,7 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>100</v>
       </c>
     </row>
@@ -822,9 +822,9 @@
         <v>14</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="9">
+        <v>59</v>
+      </c>
+      <c r="D17" s="8">
         <f>SUM(D18:D24)/7</f>
         <v>100</v>
       </c>
@@ -833,7 +833,7 @@
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>100</v>
       </c>
     </row>
@@ -841,7 +841,7 @@
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>100</v>
       </c>
     </row>
@@ -849,7 +849,7 @@
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>100</v>
       </c>
     </row>
@@ -857,7 +857,7 @@
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>100</v>
       </c>
     </row>
@@ -865,7 +865,7 @@
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>100</v>
       </c>
     </row>
@@ -873,7 +873,7 @@
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>100</v>
       </c>
     </row>
@@ -881,7 +881,7 @@
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>100</v>
       </c>
     </row>
@@ -893,18 +893,18 @@
         <v>26</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="9">
+        <v>59</v>
+      </c>
+      <c r="D25" s="8">
         <f>SUM(D26:D29)/4</f>
-        <v>75</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>100</v>
       </c>
     </row>
@@ -912,7 +912,7 @@
       <c r="B27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>100</v>
       </c>
     </row>
@@ -920,16 +920,16 @@
       <c r="B28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="7">
-        <v>100</v>
+      <c r="D28" s="6">
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="7">
-        <v>0</v>
+      <c r="D29" s="6">
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -940,9 +940,9 @@
         <v>32</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="9">
+        <v>59</v>
+      </c>
+      <c r="D30" s="8">
         <f>SUM(D31:D33)/3</f>
         <v>30</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>0</v>
       </c>
     </row>
@@ -959,7 +959,7 @@
       <c r="B32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="6">
         <v>90</v>
       </c>
     </row>
@@ -967,7 +967,7 @@
       <c r="B33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="6">
         <v>0</v>
       </c>
     </row>
@@ -979,9 +979,9 @@
         <v>37</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="9">
+        <v>59</v>
+      </c>
+      <c r="D34" s="8">
         <f>SUM(D35:D36)/2</f>
         <v>0</v>
       </c>
@@ -990,7 +990,7 @@
       <c r="B35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="6">
         <v>0</v>
       </c>
     </row>
@@ -998,7 +998,7 @@
       <c r="B36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1010,9 +1010,9 @@
         <v>41</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="9">
+        <v>59</v>
+      </c>
+      <c r="D37" s="8">
         <f>SUM(D38:D40)/3</f>
         <v>66.666666666666671</v>
       </c>
@@ -1021,7 +1021,7 @@
       <c r="B38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="6">
         <v>100</v>
       </c>
     </row>
@@ -1029,15 +1029,15 @@
       <c r="B39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="6">
         <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="7">
+        <v>79</v>
+      </c>
+      <c r="D40" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1049,9 +1049,9 @@
         <v>45</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D41" s="9">
+        <v>59</v>
+      </c>
+      <c r="D41" s="8">
         <f>SUM(D42:D45)/4</f>
         <v>0</v>
       </c>
@@ -1060,7 +1060,7 @@
       <c r="B42" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1068,7 +1068,7 @@
       <c r="B43" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1076,68 +1076,68 @@
       <c r="B44" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="7">
+        <v>80</v>
+      </c>
+      <c r="D45" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="C46" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="9">
+        <v>59</v>
+      </c>
+      <c r="D46" s="8">
         <f>SUM(D47:D49)/3</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D47" s="7">
+        <v>51</v>
+      </c>
+      <c r="D47" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D48" s="7">
+        <v>52</v>
+      </c>
+      <c r="D48" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D49" s="7">
+        <v>53</v>
+      </c>
+      <c r="D49" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="C50" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="9">
+        <v>59</v>
+      </c>
+      <c r="D50" s="8">
         <f>SUM(D51:D52)/2</f>
         <v>0</v>
       </c>
@@ -1145,128 +1145,128 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" s="3"/>
-      <c r="D51" s="10">
+      <c r="D51" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D52" s="7">
+        <v>57</v>
+      </c>
+      <c r="D52" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D53" s="9"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="C54" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="C55" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="C56" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="C57" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D57" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="C58" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D58" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="C59" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D59" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="C60" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D60" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="D60" s="8"/>
     </row>
     <row r="61" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="C61" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D61" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="D61" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Tasks + Bucket's Attachments + Update RD&T
</commit_message>
<xml_diff>
--- a/ZZ_Docs/Tasks.xlsx
+++ b/ZZ_Docs/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chalmers\2020\PPU080 Advanced computer aided design\06 - Project\PPU080_Excavator\ZZ_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8F6F32-3C65-40C7-87CF-2ECECC76BBCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D38188-28B4-40B1-8985-4E09323BECC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F51A760-8785-45A1-A29B-AFB17A55C109}"/>
   </bookViews>
@@ -690,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780EFD92-2DE3-4928-85FB-6DCD7360F672}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -897,7 +897,7 @@
       </c>
       <c r="D25" s="8">
         <f>SUM(D26:D29)/4</f>
-        <v>87.5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -921,7 +921,7 @@
         <v>29</v>
       </c>
       <c r="D28" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="D41" s="8">
         <f>SUM(D42:D45)/4</f>
-        <v>0</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1061,7 +1061,7 @@
         <v>46</v>
       </c>
       <c r="D42" s="6">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1069,7 +1069,7 @@
         <v>47</v>
       </c>
       <c r="D43" s="6">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1077,7 +1077,7 @@
         <v>48</v>
       </c>
       <c r="D44" s="6">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1085,7 +1085,7 @@
         <v>80</v>
       </c>
       <c r="D45" s="6">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1100,7 +1100,7 @@
       </c>
       <c r="D46" s="8">
         <f>SUM(D47:D49)/3</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1116,7 +1116,7 @@
         <v>52</v>
       </c>
       <c r="D48" s="6">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Tasks Update + Personal Files
</commit_message>
<xml_diff>
--- a/ZZ_Docs/Tasks.xlsx
+++ b/ZZ_Docs/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chalmers\2020\PPU080 Advanced computer aided design\06 - Project\PPU080_Excavator\ZZ_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA73147B-9AE8-4AAD-B495-7CF38038D967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11569DD-3F67-4618-963C-BB66CF9E5A93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F51A760-8785-45A1-A29B-AFB17A55C109}"/>
   </bookViews>
@@ -694,7 +694,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -986,7 +986,7 @@
       </c>
       <c r="D34" s="8">
         <f>SUM(D35:D36)/2</f>
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -994,7 +994,7 @@
         <v>38</v>
       </c>
       <c r="D35" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="D37" s="8">
         <f>SUM(D38:D40)/3</f>
-        <v>66.666666666666671</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1041,7 +1041,7 @@
         <v>79</v>
       </c>
       <c r="D40" s="6">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="D41" s="8">
         <f>SUM(D42:D46)/5</f>
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1088,7 +1088,7 @@
         <v>81</v>
       </c>
       <c r="D45" s="6">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1096,7 +1096,7 @@
         <v>80</v>
       </c>
       <c r="D46" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Screws : Done ! And constraints hiding
</commit_message>
<xml_diff>
--- a/ZZ_Docs/Tasks.xlsx
+++ b/ZZ_Docs/Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chalmers\2020\PPU080 Advanced computer aided design\06 - Project\PPU080_Excavator\ZZ_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11569DD-3F67-4618-963C-BB66CF9E5A93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA88274-8539-48FC-825A-A41679D176D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F51A760-8785-45A1-A29B-AFB17A55C109}"/>
   </bookViews>
@@ -694,7 +694,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -955,7 +955,7 @@
         <v>33</v>
       </c>
       <c r="D31" s="6">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -963,7 +963,7 @@
         <v>34</v>
       </c>
       <c r="D32" s="6">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="D41" s="8">
         <f>SUM(D42:D46)/5</f>
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1088,7 +1088,7 @@
         <v>81</v>
       </c>
       <c r="D45" s="6">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D47" s="8">
         <f>SUM(D48:D50)/3</f>
-        <v>66.666666666666671</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1135,7 +1135,7 @@
         <v>53</v>
       </c>
       <c r="D50" s="6">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="D51" s="8">
         <f>SUM(D52:D53)/2</f>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1168,7 +1168,7 @@
         <v>57</v>
       </c>
       <c r="D53" s="6">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>